<commit_message>
Added: after contract termination
</commit_message>
<xml_diff>
--- a/error.xlsx
+++ b/error.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ERROR_LIST" sheetId="1" state="visible" r:id="rId3"/>
@@ -14,6 +14,7 @@
     <sheet name="Failed Order tracker" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="BMC - Ricket" sheetId="5" state="visible" r:id="rId7"/>
     <sheet name="Production_tracker_template" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="Solution" sheetId="7" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="361">
   <si>
     <t xml:space="preserve">Order_type</t>
   </si>
@@ -153,11 +154,14 @@
     <t xml:space="preserve">ChangeSim</t>
   </si>
   <si>
+    <t xml:space="preserve">400 :: Invalid Patch for Path:/identities for operation:replace. The Identity supplied in Where clause is not associated with this device. :: NCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nothing to do, duplicate order </t>
+  </si>
+  <si>
     <t xml:space="preserve">400 :: Invalid Patch for Path:/identities for operation:replace. The Identity supplied in 
 Where clause is not associated with this device. :: NCC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nothing to do, duplicate order </t>
   </si>
   <si>
     <t xml:space="preserve">AddServiceToNewAccount</t>
@@ -478,9 +482,6 @@
     <t xml:space="preserve">manually delete from HLR</t>
   </si>
   <si>
-    <t xml:space="preserve">SC0001 :: customer not valid :: Loyalty Management</t>
-  </si>
-  <si>
     <t xml:space="preserve">SC0007 :: Customer Already Exists :: Loyalty Management error in LMS 
 -the cust already exist in DB Error from HLR</t>
   </si>
@@ -496,6 +497,9 @@
   </si>
   <si>
     <t xml:space="preserve">IVR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SC0001 :: customer not valid :: Loyalty Management</t>
   </si>
   <si>
     <t xml:space="preserve">The object: imsi=636020100000100,dc=IMSI,dc=C-NTDB - was not found in the Database.</t>
@@ -1210,7 +1214,115 @@
     <t xml:space="preserve">Asnake</t>
   </si>
   <si>
-    <t xml:space="preserve">INC000000043462</t>
+    <t xml:space="preserve">INC000000043844</t>
+  </si>
+  <si>
+    <t xml:space="preserve">order_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State_reason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bulk rettry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fill SID into 
+/home/svc-bss-pam@safaricomet.net/OPS/ORDER-RETRY/orderidsuborderid.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo su -l -c 'nohup sh -x /home/svc-bss-pam@safaricomet.net/OPS/ORDER-RETRY/ORDER_RETRY.sh &amp; 2&gt; /dev/null'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">onoarding
+Addservice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subscriber creation in LMS
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in LMS DB,  the entry should be empty; so remove from DB before provisioning another customer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">then retry order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo su -l -c 'nohup sh -x /home/akshay.pp@safaricomet.net/Scripts/LMS_ORDER_RETRY/LMS_ORDER_RETRY.sh &amp; 2&gt; /dev/null'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COM-001:Internal Error: error in forming tp request
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400 :: Cannot parse "01-01-1960": Illegal instant due to time zone offset transition </t>
+  </si>
+  <si>
+    <t xml:space="preserve">updateLanguage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo su -l -c 'nohup sh -x /home/akshay.pp@safaricomet.net/scripts/lms_order_retry/lms_order_retry.sh &amp; 2&gt; /dev/null'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to fire postman to fill onboarding entry -api</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unable to find base plan id in CM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check 360 view OCS status is active billing status is active, 
+check in WKN_UPC--SM_SUBSCRIPTION_07 --&gt;07 is the last MSISDN 
+status is D make it A (deactive/active)
+SEQ_ID is null make base plan id in place of null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">then retry the order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desc: Fetch Service Registry in SOM
+Reason: 404 Not found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WKN_SOM--&gt;service_registry_item table--find 
+externalserviceid='251703099300' and status is inactive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skip the order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reducing logs file theory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              from backup directory
+All modules – Delete &gt;10-15 days logs
+PRM – zip all bup logs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from Current directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM - we will nullify current logs
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">onboarding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provisioning in SOM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cshould be AUC:encKey provided.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reinitiate the order using postman, using api calling to SOM, it should be provisioned</t>
   </si>
 </sst>
 </file>
@@ -1222,7 +1334,7 @@
     <numFmt numFmtId="165" formatCode="hh:mm:ss\ AM/PM"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1346,8 +1458,42 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10.5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1382,6 +1528,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF38"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF38"/>
       </patternFill>
     </fill>
   </fills>
@@ -1609,7 +1761,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="88">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1894,10 +2046,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1923,6 +2071,46 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="7" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2126,8 +2314,8 @@
   </sheetPr>
   <dimension ref="A1:XFD94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2313,7 +2501,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="33.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>33</v>
       </c>
@@ -2329,292 +2517,292 @@
     </row>
     <row r="15" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="D15" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="C16" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
+      <c r="D16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="4" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="9" t="s">
+      <c r="C17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
+    <row r="18" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="C18" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="95.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
+      <c r="D18" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="95.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B19" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="C19" s="6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="D19" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="4" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="C20" s="6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+      <c r="D20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="6" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="9" t="s">
+      <c r="C21" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="4" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="83.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="4" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="83.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="32.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
+      <c r="D23" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="10" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="32.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="4" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4" t="s">
+    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="4" t="s">
+    <row r="27" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="4" t="s">
+      <c r="C27" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>70</v>
+      <c r="C29" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31" s="4"/>
+        <v>72</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="C31" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="32.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6" t="s">
+    <row r="33" customFormat="false" ht="32.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B33" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" s="14" customFormat="true" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6" t="s">
+      <c r="D33" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="D34" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" s="14" customFormat="true" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="B35" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="XFC34" s="1"/>
-      <c r="XFD34" s="1"/>
-    </row>
-    <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>78</v>
+      <c r="C35" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="XFC35" s="1"/>
+      <c r="XFD35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>79</v>
@@ -2623,266 +2811,266 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" s="15" customFormat="true" ht="48.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="4" t="s">
         <v>80</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="XFC37" s="1"/>
-      <c r="XFD37" s="1"/>
-    </row>
-    <row r="38" customFormat="false" ht="48.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
+    </row>
+    <row r="38" s="15" customFormat="true" ht="48.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="C38" s="6" t="s">
         <v>81</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
+      <c r="XFC38" s="1"/>
+      <c r="XFD38" s="1"/>
+    </row>
+    <row r="39" customFormat="false" ht="48.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" s="4" t="s">
+      <c r="D40" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="6" t="s">
+    </row>
+    <row r="41" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="C41" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="63.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
+    <row r="42" customFormat="false" ht="63.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D41" s="6" t="s">
+      <c r="C42" s="4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="48.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="s">
+      <c r="D42" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="48.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B43" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B43" s="4"/>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="6" t="s">
         <v>89</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="63.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="6" t="s">
+    <row r="44" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="4"/>
+      <c r="C44" s="8" t="s">
         <v>90</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
-        <v>60</v>
-      </c>
+    <row r="45" customFormat="false" ht="63.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4"/>
       <c r="B45" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="4"/>
+      <c r="D45" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B46" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D46" s="9" t="s">
+    </row>
+    <row r="47" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D47" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" s="4" t="s">
+    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4" t="s">
+      <c r="D48" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D48" s="6" t="s">
+      <c r="C49" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="32.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="6" t="s">
+    <row r="50" customFormat="false" ht="32.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C50" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D49" s="9" t="s">
+      <c r="D50" s="9" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C51" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D51" s="4" t="s">
+    </row>
+    <row r="52" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B52" s="5" t="s">
+    <row r="53" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C52" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D52" s="4" t="s">
+      <c r="B53" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B53" s="6" t="s">
+    <row r="54" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C53" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="6" t="s">
         <v>106</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4"/>
+      <c r="A55" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="C55" s="4" t="s">
         <v>107</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C56" s="6" t="s">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4" t="s">
         <v>108</v>
       </c>
       <c r="D56" s="4" t="s">
@@ -2890,198 +3078,200 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="4" t="s">
-        <v>53</v>
+      <c r="A57" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="6" t="s">
         <v>109</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>110</v>
+        <v>21</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C59" s="6" t="s">
-        <v>112</v>
+      <c r="C59" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="6" t="s">
         <v>113</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>58</v>
+      <c r="D61" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C62" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D62" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D62" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D63" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D63" s="9" t="s">
+    </row>
+    <row r="64" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D64" s="9" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="C65" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D65" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C66" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="4" t="s">
+      <c r="C67" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B67" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C67" s="4" t="s">
+      <c r="B68" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="C68" s="4" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="68" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="6" t="s">
+      <c r="D68" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D69" s="6" t="s">
+      <c r="C70" s="6" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="70" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C70" s="4" t="s">
+      <c r="D70" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D70" s="6"/>
     </row>
     <row r="71" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="4" t="s">
@@ -3097,7 +3287,7 @@
     </row>
     <row r="72" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="6" t="s">
@@ -3127,21 +3317,21 @@
         <v>138</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D75" s="4"/>
     </row>
@@ -3153,7 +3343,7 @@
         <v>7</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>21</v>
@@ -3161,44 +3351,44 @@
     </row>
     <row r="77" customFormat="false" ht="33.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="48.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="17.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="17.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3209,22 +3399,22 @@
         <v>7</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D80" s="4"/>
     </row>
     <row r="81" customFormat="false" ht="17.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="17.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3235,21 +3425,21 @@
         <v>7</v>
       </c>
       <c r="C82" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>21</v>
@@ -3263,32 +3453,32 @@
         <v>7</v>
       </c>
       <c r="C84" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="18" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C85" s="18"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C89" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B90" s="19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3330,15 +3520,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="22" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="23" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F1" s="23"/>
       <c r="G1" s="23"/>
@@ -3347,15 +3537,15 @@
     </row>
     <row r="2" customFormat="false" ht="67.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="25" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D2" s="25"/>
       <c r="E2" s="26" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F2" s="26"/>
       <c r="G2" s="26"/>
@@ -3364,15 +3554,15 @@
     </row>
     <row r="3" customFormat="false" ht="46" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B3" s="24"/>
       <c r="C3" s="25" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="26" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F3" s="26"/>
       <c r="G3" s="26"/>
@@ -3385,11 +3575,11 @@
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="27" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D4" s="27"/>
       <c r="E4" s="26" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F4" s="26"/>
       <c r="G4" s="26"/>
@@ -3398,15 +3588,15 @@
     </row>
     <row r="5" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="24" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="27" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="28" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
@@ -3415,15 +3605,15 @@
     </row>
     <row r="6" customFormat="false" ht="32.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="24" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B6" s="24"/>
       <c r="C6" s="27" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="26" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
@@ -3432,15 +3622,15 @@
     </row>
     <row r="7" customFormat="false" ht="32.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="24" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="27" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="26" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
@@ -3449,15 +3639,15 @@
     </row>
     <row r="8" customFormat="false" ht="32.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="27" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D8" s="27"/>
       <c r="E8" s="26" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
@@ -3466,15 +3656,15 @@
     </row>
     <row r="9" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="27" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="26" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F9" s="26"/>
       <c r="G9" s="26"/>
@@ -3483,15 +3673,15 @@
     </row>
     <row r="10" customFormat="false" ht="32.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="24" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B10" s="24"/>
       <c r="C10" s="27" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F10" s="26"/>
       <c r="G10" s="26"/>
@@ -3500,15 +3690,15 @@
     </row>
     <row r="11" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="24" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B11" s="24"/>
       <c r="C11" s="27" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="26" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
@@ -3519,11 +3709,11 @@
       <c r="A12" s="24"/>
       <c r="B12" s="24"/>
       <c r="C12" s="27" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="26" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="26"/>
@@ -3532,15 +3722,15 @@
     </row>
     <row r="13" customFormat="false" ht="32.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="24" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B13" s="24"/>
       <c r="C13" s="27" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="26" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F13" s="26"/>
       <c r="G13" s="26"/>
@@ -3560,15 +3750,15 @@
     </row>
     <row r="15" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B15" s="29"/>
       <c r="C15" s="30" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D15" s="30"/>
       <c r="E15" s="31" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F15" s="31"/>
       <c r="G15" s="31"/>
@@ -3577,15 +3767,15 @@
     </row>
     <row r="16" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B16" s="29"/>
       <c r="C16" s="30" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D16" s="30"/>
       <c r="E16" s="31" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F16" s="31"/>
       <c r="G16" s="31"/>
@@ -3600,7 +3790,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="33" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="33"/>
@@ -3714,22 +3904,22 @@
     </row>
     <row r="32" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="34" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C32" s="34"/>
       <c r="D32" s="34"/>
     </row>
     <row r="34" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D34" s="19" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="79.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="35" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B35" s="35"/>
       <c r="C35" s="35"/>
@@ -3749,77 +3939,77 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="19" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="19" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="19" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="19" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="19" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="19" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="19" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="19" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="19" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="19" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3827,52 +4017,52 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -3963,15 +4153,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="22" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="23" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F1" s="23"/>
       <c r="G1" s="23"/>
@@ -3980,15 +4170,15 @@
     </row>
     <row r="2" customFormat="false" ht="98.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="25" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D2" s="25"/>
       <c r="E2" s="37" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F2" s="37"/>
       <c r="G2" s="37"/>
@@ -3997,11 +4187,11 @@
     </row>
     <row r="3" customFormat="false" ht="50.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B3" s="24"/>
       <c r="C3" s="25" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="38" t="str">
@@ -4010,7 +4200,7 @@
 BMC ID: INC000000028097 (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
         <v>Hi  Biruk, 
 PFB provisioning order failed at NCC for W/A
-BMC ID: INC000000028097 (08-09-2024)</v>
+BMC ID: INC000000028097 (27-09-2024)</v>
       </c>
       <c r="F3" s="38"/>
       <c r="G3" s="38"/>
@@ -4019,11 +4209,11 @@
     </row>
     <row r="4" customFormat="false" ht="50.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="25" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D4" s="25"/>
       <c r="E4" s="38" t="str">
@@ -4032,7 +4222,7 @@
 BMC ID: INC000000028097 (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
         <v>Hi  Biruk, 
 PFB provisioning order failed at NCC for W/A
-BMC ID: INC000000028097 (08-09-2024)</v>
+BMC ID: INC000000028097 (27-09-2024)</v>
       </c>
       <c r="F4" s="38"/>
       <c r="G4" s="38"/>
@@ -4045,7 +4235,7 @@
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="27" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="38" t="str">
@@ -4054,7 +4244,7 @@
 BMC ID: INC000000028097 (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
         <v>Hi  Biruk, 
 PFB UpdatLangiage order failed at NCC for W/A
-BMC ID: INC000000028097 (08-09-2024)</v>
+BMC ID: INC000000028097 (27-09-2024)</v>
       </c>
       <c r="F5" s="38"/>
       <c r="G5" s="38"/>
@@ -4063,11 +4253,11 @@
     </row>
     <row r="6" customFormat="false" ht="56.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="24" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B6" s="24"/>
       <c r="C6" s="27" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="38" t="str">
@@ -4076,7 +4266,7 @@
 BMC ID: INC000000028097 (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
         <v>Hi  Biruk, 
 PFB ChangeSim order failed at NCC for W/A
-BMC ID: INC000000028097 (08-09-2024)</v>
+BMC ID: INC000000028097 (27-09-2024)</v>
       </c>
       <c r="F6" s="38"/>
       <c r="G6" s="38"/>
@@ -4085,11 +4275,11 @@
     </row>
     <row r="7" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="27" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="38" t="str">
@@ -4098,7 +4288,7 @@
 BMC ID: INC000000028097 (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
         <v>Hi  Biruk, 
 PFB Lifecyclesync Termination order failed at NCC for W/A
-BMC ID: INC000000028097 (08-09-2024)</v>
+BMC ID: INC000000028097 (27-09-2024)</v>
       </c>
       <c r="F7" s="38"/>
       <c r="G7" s="38"/>
@@ -4107,11 +4297,11 @@
     </row>
     <row r="8" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="24" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="27" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D8" s="27"/>
       <c r="E8" s="38" t="str">
@@ -4120,7 +4310,7 @@
 BMC ID: INC000000028097 (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
         <v>Hi  Biruk, 
 PFB AddSubscription order failed at NCC for W/A
-BMC ID: INC000000028097 (08-09-2024)</v>
+BMC ID: INC000000028097 (27-09-2024)</v>
       </c>
       <c r="F8" s="38"/>
       <c r="G8" s="38"/>
@@ -4129,11 +4319,11 @@
     </row>
     <row r="9" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="27" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="38" t="str">
@@ -4142,7 +4332,7 @@
 BMC ID: INC000000028097 (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
         <v>Hi  Biruk, 
 PFB ChangeSUbscription order failed at NCC for W/A
-BMC ID: INC000000028097 (08-09-2024)</v>
+BMC ID: INC000000028097 (27-09-2024)</v>
       </c>
       <c r="F9" s="38"/>
       <c r="G9" s="38"/>
@@ -4151,11 +4341,11 @@
     </row>
     <row r="10" customFormat="false" ht="64.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="24" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B10" s="24"/>
       <c r="C10" s="27" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="38" t="str">
@@ -4164,7 +4354,7 @@
 BMC ID: INC000000028097 (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
         <v>Hi  Biruk, 
 PFB TerminateService order failed at NCC for W/A
-BMC ID: INC000000028097 (08-09-2024)</v>
+BMC ID: INC000000028097 (27-09-2024)</v>
       </c>
       <c r="F10" s="38"/>
       <c r="G10" s="38"/>
@@ -4173,11 +4363,11 @@
     </row>
     <row r="11" customFormat="false" ht="39.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="24" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B11" s="24"/>
       <c r="C11" s="27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="38" t="str">
@@ -4186,7 +4376,7 @@
 BMC ID: INC000000028097 (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
         <v>Hi  Biruk, 
 PFB ConnectionMigration order failed at ERP for W/A
-BMC ID: INC000000028097 (08-09-2024)</v>
+BMC ID: INC000000028097 (27-09-2024)</v>
       </c>
       <c r="F11" s="38"/>
       <c r="G11" s="38"/>
@@ -4197,11 +4387,11 @@
       <c r="A12" s="24"/>
       <c r="B12" s="24"/>
       <c r="C12" s="27" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="37" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
@@ -4210,15 +4400,15 @@
     </row>
     <row r="13" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="24" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B13" s="24"/>
       <c r="C13" s="27" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="37" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
@@ -4229,11 +4419,11 @@
       <c r="A14" s="24"/>
       <c r="B14" s="24"/>
       <c r="C14" s="27" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D14" s="27"/>
       <c r="E14" s="37" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
@@ -4242,11 +4432,11 @@
     </row>
     <row r="15" customFormat="false" ht="39.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="24" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B15" s="24"/>
       <c r="C15" s="27" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="37"/>
@@ -4257,15 +4447,15 @@
     </row>
     <row r="16" customFormat="false" ht="36.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="24" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B16" s="24"/>
       <c r="C16" s="27" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D16" s="27"/>
       <c r="E16" s="37" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
@@ -4274,15 +4464,15 @@
     </row>
     <row r="17" customFormat="false" ht="121.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B17" s="24"/>
       <c r="C17" s="27" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D17" s="27"/>
       <c r="E17" s="37" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
@@ -4291,15 +4481,15 @@
     </row>
     <row r="18" customFormat="false" ht="121.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="24" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B18" s="24"/>
       <c r="C18" s="39" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D18" s="39"/>
       <c r="E18" s="37" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F18" s="37"/>
       <c r="G18" s="37"/>
@@ -4310,11 +4500,11 @@
       <c r="A19" s="24"/>
       <c r="B19" s="24"/>
       <c r="C19" s="39" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D19" s="39"/>
       <c r="E19" s="37" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F19" s="37"/>
       <c r="G19" s="37"/>
@@ -4325,11 +4515,11 @@
       <c r="A20" s="24"/>
       <c r="B20" s="24"/>
       <c r="C20" s="39" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D20" s="39"/>
       <c r="E20" s="37" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F20" s="37"/>
       <c r="G20" s="37"/>
@@ -4340,11 +4530,11 @@
       <c r="A21" s="24"/>
       <c r="B21" s="24"/>
       <c r="C21" s="39" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D21" s="39"/>
       <c r="E21" s="37" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F21" s="37"/>
       <c r="G21" s="37"/>
@@ -4353,15 +4543,15 @@
     </row>
     <row r="22" customFormat="false" ht="32.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="29" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B22" s="29"/>
       <c r="C22" s="30" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D22" s="30"/>
       <c r="E22" s="40" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F22" s="40"/>
       <c r="G22" s="40"/>
@@ -4370,11 +4560,11 @@
     </row>
     <row r="23" customFormat="false" ht="32.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="29" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B23" s="29"/>
       <c r="C23" s="41" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D23" s="41"/>
       <c r="E23" s="42" t="str">
@@ -4383,7 +4573,7 @@
 BMC ID: INC000000028097 (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
         <v>Hi  Biruk, 
 PFB NumberRecycle order failed at HLR for W/A
-BMC ID: INC000000028097 (08-09-2024)</v>
+BMC ID: INC000000028097 (27-09-2024)</v>
       </c>
       <c r="F23" s="42"/>
       <c r="G23" s="42"/>
@@ -4489,7 +4679,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="43" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -4501,13 +4691,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="44" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B2" s="44"/>
       <c r="C2" s="44"/>
       <c r="D2" s="44"/>
       <c r="E2" s="44" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
@@ -4515,13 +4705,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="44" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
       <c r="D3" s="44"/>
       <c r="E3" s="44" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F3" s="44"/>
       <c r="G3" s="44"/>
@@ -4529,13 +4719,13 @@
     </row>
     <row r="4" customFormat="false" ht="34.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="45" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B4" s="45"/>
       <c r="C4" s="45"/>
       <c r="D4" s="45"/>
       <c r="E4" s="44" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F4" s="44"/>
       <c r="G4" s="44"/>
@@ -4543,13 +4733,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="44" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
       <c r="D5" s="44"/>
       <c r="E5" s="44" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F5" s="44"/>
       <c r="G5" s="44"/>
@@ -4557,13 +4747,13 @@
     </row>
     <row r="6" customFormat="false" ht="23.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="46" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B6" s="46"/>
       <c r="C6" s="46"/>
       <c r="D6" s="46"/>
       <c r="E6" s="44" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F6" s="44"/>
       <c r="G6" s="44"/>
@@ -4571,12 +4761,12 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="33" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
@@ -4608,7 +4798,7 @@
     </row>
     <row r="13" customFormat="false" ht="23.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="47" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B13" s="47"/>
       <c r="C13" s="47"/>
@@ -4620,7 +4810,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="48" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="48"/>
@@ -4632,12 +4822,12 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="19" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="49" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B17" s="49"/>
       <c r="C17" s="49"/>
@@ -4723,7 +4913,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4735,13 +4925,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C1" s="53" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4750,260 +4940,260 @@
       </c>
       <c r="B2" s="52" t="str">
         <f aca="true">CONCATENATE("ChangeSim Order failure at NCC  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>ChangeSim Order failure at NCC  (08-09-2024)</v>
+        <v>ChangeSim Order failure at NCC  (27-09-2024)</v>
       </c>
       <c r="C2" s="55" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="54" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B3" s="52" t="str">
         <f aca="true">CONCATENATE("Requested to refresh SM -  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>Requested to refresh SM -  (08-09-2024)</v>
+        <v>Requested to refresh SM -  (27-09-2024)</v>
       </c>
       <c r="C3" s="56" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="54" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B4" s="52" t="str">
         <f aca="true">CONCATENATE("Fnf Order Failure at NCC  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>Fnf Order Failure at NCC  (08-09-2024)</v>
+        <v>Fnf Order Failure at NCC  (27-09-2024)</v>
       </c>
       <c r="C4" s="55" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="54" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B5" s="52" t="str">
         <f aca="true">CONCATENATE("ConnectionMigration Failure at ERP  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>ConnectionMigration Failure at ERP  (08-09-2024)</v>
+        <v>ConnectionMigration Failure at ERP  (27-09-2024)</v>
       </c>
       <c r="C5" s="57" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="54" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C6" s="58" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="25.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="54"/>
       <c r="B7" s="59" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C7" s="58" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="54"/>
       <c r="B8" s="52" t="str">
         <f aca="true">CONCATENATE("Prepaid Provisioning Failures from NCC  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>Prepaid Provisioning Failures from NCC  (08-09-2024)</v>
+        <v>Prepaid Provisioning Failures from NCC  (27-09-2024)</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="54" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B9" s="52" t="str">
         <f aca="true">CONCATENATE("Postpaid Provisioning Failures in Linking device at NCC  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>Postpaid Provisioning Failures in Linking device at NCC  (08-09-2024)</v>
+        <v>Postpaid Provisioning Failures in Linking device at NCC  (27-09-2024)</v>
       </c>
       <c r="C9" s="60" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="54" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B10" s="52" t="str">
         <f aca="true">CONCATENATE("Provisioning order failures at ERP  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>Provisioning order failures at ERP  (08-09-2024)</v>
+        <v>Provisioning order failures at ERP  (27-09-2024)</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="54" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B11" s="52" t="str">
         <f aca="true">CONCATENATE("Provisioning order failures at SND  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>Provisioning order failures at SND  (08-09-2024)</v>
+        <v>Provisioning order failures at SND  (27-09-2024)</v>
       </c>
       <c r="C11" s="60" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="54"/>
       <c r="B12" s="52" t="str">
         <f aca="true">CONCATENATE("ChangeSubscription failure at NCC  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>ChangeSubscription failure at NCC  (08-09-2024)</v>
+        <v>ChangeSubscription failure at NCC  (27-09-2024)</v>
       </c>
       <c r="C12" s="60" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="54"/>
       <c r="B13" s="52" t="str">
         <f aca="true">CONCATENATE("Linebarring Failed Orders at NCC  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>Linebarring Failed Orders at NCC  (08-09-2024)</v>
+        <v>Linebarring Failed Orders at NCC  (27-09-2024)</v>
       </c>
       <c r="C13" s="60" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="54"/>
       <c r="B14" s="52" t="str">
         <f aca="true">CONCATENATE("Linebarring Failed Orders at HLR  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>Linebarring Failed Orders at HLR  (08-09-2024)</v>
+        <v>Linebarring Failed Orders at HLR  (27-09-2024)</v>
       </c>
       <c r="C14" s="60" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="54"/>
       <c r="B15" s="52" t="str">
         <f aca="true">CONCATENATE("LineUnBarring Failed Orders at NCC  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>LineUnBarring Failed Orders at NCC  (08-09-2024)</v>
+        <v>LineUnBarring Failed Orders at NCC  (27-09-2024)</v>
       </c>
       <c r="C15" s="60" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="54" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B16" s="52" t="str">
         <f aca="true">CONCATENATE("TerminateService Failures – NCC  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>TerminateService Failures – NCC  (08-09-2024)</v>
+        <v>TerminateService Failures – NCC  (27-09-2024)</v>
       </c>
       <c r="C16" s="60" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="54" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B17" s="52" t="str">
         <f aca="true">CONCATENATE("TransferOfService Failures – NCC  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>TransferOfService Failures – NCC  (08-09-2024)</v>
+        <v>TransferOfService Failures – NCC  (27-09-2024)</v>
       </c>
       <c r="C17" s="60" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="54"/>
       <c r="B18" s="52" t="str">
         <f aca="true">CONCATENATE("SoftBarring Order Failure at NCC  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>SoftBarring Order Failure at NCC  (08-09-2024)</v>
+        <v>SoftBarring Order Failure at NCC  (27-09-2024)</v>
       </c>
       <c r="C18" s="57" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="54"/>
       <c r="B19" s="52" t="str">
         <f aca="true">CONCATENATE("HardUnbarring Order Failure at NCC  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>HardUnbarring Order Failure at NCC  (08-09-2024)</v>
+        <v>HardUnbarring Order Failure at NCC  (27-09-2024)</v>
       </c>
       <c r="C19" s="57" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="54"/>
       <c r="B20" s="52" t="str">
         <f aca="true">CONCATENATE("Lifecyclesync Termination failure at HLR  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>Lifecyclesync Termination failure at HLR  (08-09-2024)</v>
+        <v>Lifecyclesync Termination failure at HLR  (27-09-2024)</v>
       </c>
       <c r="C20" s="57" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="54" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B21" s="52" t="str">
         <f aca="true">CONCATENATE("UpdateOobFlag order failure  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>UpdateOobFlag order failure  (08-09-2024)</v>
+        <v>UpdateOobFlag order failure  (27-09-2024)</v>
       </c>
       <c r="C21" s="57" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="54"/>
       <c r="B22" s="52" t="str">
         <f aca="true">CONCATENATE("INC000000069223|| Language update and Change SIM active failure cases  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>INC000000069223|| Language update and Change SIM active failure cases  (08-09-2024)</v>
+        <v>INC000000069223|| Language update and Change SIM active failure cases  (27-09-2024)</v>
       </c>
       <c r="C22" s="60" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="54" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B23" s="52" t="str">
         <f aca="true">CONCATENATE("SoftBarring and SoftUnbarring Order Failures - NCC  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>SoftBarring and SoftUnbarring Order Failures - NCC  (08-09-2024)</v>
+        <v>SoftBarring and SoftUnbarring Order Failures - NCC  (27-09-2024)</v>
       </c>
       <c r="C23" s="60" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="54"/>
       <c r="B24" s="52" t="str">
         <f aca="true">CONCATENATE("NumberRecycle failure at HLR  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>NumberRecycle failure at HLR  (08-09-2024)</v>
+        <v>NumberRecycle failure at HLR  (27-09-2024)</v>
       </c>
       <c r="C24" s="55" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="54"/>
       <c r="B25" s="52" t="str">
         <f aca="true">CONCATENATE("NumberRecycle failure at NCC  (",TEXT(TODAY(),"dd-mm-yyyy"),")")</f>
-        <v>NumberRecycle failure at NCC  (08-09-2024)</v>
+        <v>NumberRecycle failure at NCC  (27-09-2024)</v>
       </c>
       <c r="C25" s="55" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5055,8 +5245,8 @@
   </sheetPr>
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5077,64 +5267,64 @@
   <sheetData>
     <row r="1" customFormat="false" ht="64.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="63" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B1" s="64" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C1" s="63" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D1" s="65" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E1" s="66" t="s">
         <v>14</v>
       </c>
       <c r="F1" s="65" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G1" s="66" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H1" s="65" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="I1" s="65" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="J1" s="65" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="K1" s="66" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="L1" s="64" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="M1" s="66" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="N1" s="65" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="O1" s="67" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="P1" s="65" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="Q1" s="67" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="R1" s="67" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="S1" s="67" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="2" s="71" customFormat="true" ht="18.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="18.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="68" t="n">
         <f aca="false">B5</f>
         <v>45366.3194444444</v>
@@ -5185,7 +5375,7 @@
       <c r="O2" s="69"/>
       <c r="P2" s="68" t="str">
         <f aca="false">B19</f>
-        <v>INC000000043462</v>
+        <v>INC000000043844</v>
       </c>
       <c r="Q2" s="69"/>
       <c r="R2" s="69"/>
@@ -5202,171 +5392,171 @@
     </row>
     <row r="5" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="36" t="s">
-        <v>296</v>
-      </c>
-      <c r="B5" s="72" t="n">
+        <v>297</v>
+      </c>
+      <c r="B5" s="71" t="n">
         <v>45366.3194444444</v>
       </c>
-      <c r="C5" s="72"/>
+      <c r="C5" s="71"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="36" t="s">
-        <v>298</v>
-      </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
+        <v>299</v>
+      </c>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="36" t="s">
-        <v>314</v>
-      </c>
-      <c r="B7" s="74" t="s">
         <v>315</v>
       </c>
-      <c r="C7" s="74"/>
+      <c r="B7" s="73" t="s">
+        <v>316</v>
+      </c>
+      <c r="C7" s="73"/>
       <c r="I7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="36" t="s">
-        <v>316</v>
-      </c>
-      <c r="B8" s="74" t="s">
         <v>317</v>
       </c>
-      <c r="C8" s="74"/>
-      <c r="D8" s="75"/>
+      <c r="B8" s="73" t="s">
+        <v>318</v>
+      </c>
+      <c r="C8" s="73"/>
+      <c r="D8" s="74"/>
     </row>
     <row r="9" customFormat="false" ht="14.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="36" t="s">
-        <v>318</v>
-      </c>
-      <c r="B9" s="74" t="s">
         <v>319</v>
       </c>
-      <c r="C9" s="74"/>
+      <c r="B9" s="73" t="s">
+        <v>320</v>
+      </c>
+      <c r="C9" s="73"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="36" t="s">
-        <v>301</v>
-      </c>
-      <c r="B10" s="74" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="74" t="s">
-        <v>84</v>
+        <v>302</v>
+      </c>
+      <c r="B10" s="73" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="36" t="s">
-        <v>302</v>
-      </c>
-      <c r="B11" s="76" t="s">
-        <v>320</v>
-      </c>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="77"/>
+        <v>303</v>
+      </c>
+      <c r="B11" s="75" t="s">
+        <v>321</v>
+      </c>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76"/>
     </row>
     <row r="12" customFormat="false" ht="14.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="36" t="s">
-        <v>303</v>
-      </c>
-      <c r="B12" s="74" t="s">
-        <v>321</v>
-      </c>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
+        <v>304</v>
+      </c>
+      <c r="B12" s="73" t="s">
+        <v>322</v>
+      </c>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
       <c r="F12" s="33"/>
     </row>
     <row r="13" customFormat="false" ht="19.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="36" t="s">
-        <v>304</v>
-      </c>
-      <c r="B13" s="74" t="s">
-        <v>322</v>
-      </c>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
+        <v>305</v>
+      </c>
+      <c r="B13" s="73" t="s">
+        <v>323</v>
+      </c>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
       <c r="N13" s="19"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="36" t="s">
-        <v>323</v>
-      </c>
-      <c r="B14" s="74" t="s">
         <v>324</v>
       </c>
-      <c r="C14" s="74"/>
+      <c r="B14" s="73" t="s">
+        <v>325</v>
+      </c>
+      <c r="C14" s="73"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="36" t="s">
-        <v>306</v>
-      </c>
-      <c r="B15" s="77"/>
-      <c r="C15" s="77"/>
+        <v>307</v>
+      </c>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="36" t="s">
-        <v>307</v>
-      </c>
-      <c r="B16" s="74" t="s">
-        <v>325</v>
-      </c>
-      <c r="C16" s="74"/>
+        <v>308</v>
+      </c>
+      <c r="B16" s="73" t="s">
+        <v>326</v>
+      </c>
+      <c r="C16" s="73"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="36" t="s">
-        <v>308</v>
-      </c>
-      <c r="B17" s="74" t="s">
-        <v>326</v>
-      </c>
-      <c r="C17" s="74"/>
+        <v>309</v>
+      </c>
+      <c r="B17" s="73" t="s">
+        <v>327</v>
+      </c>
+      <c r="C17" s="73"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="36" t="s">
-        <v>309</v>
-      </c>
-      <c r="B18" s="77"/>
-      <c r="C18" s="77"/>
+        <v>310</v>
+      </c>
+      <c r="B18" s="76"/>
+      <c r="C18" s="76"/>
     </row>
     <row r="19" customFormat="false" ht="15.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="36" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B19" s="48" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C19" s="48"/>
     </row>
     <row r="20" customFormat="false" ht="15.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="36" t="s">
-        <v>311</v>
-      </c>
-      <c r="B20" s="77"/>
-      <c r="C20" s="77"/>
-      <c r="Q20" s="78"/>
+        <v>312</v>
+      </c>
+      <c r="B20" s="76"/>
+      <c r="C20" s="76"/>
+      <c r="Q20" s="77"/>
     </row>
     <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="36" t="s">
-        <v>312</v>
-      </c>
-      <c r="B21" s="77"/>
-      <c r="C21" s="77"/>
-      <c r="J21" s="78"/>
+        <v>313</v>
+      </c>
+      <c r="B21" s="76"/>
+      <c r="C21" s="76"/>
+      <c r="J21" s="77"/>
     </row>
     <row r="22" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="36" t="s">
-        <v>313</v>
-      </c>
-      <c r="B22" s="77"/>
-      <c r="C22" s="77"/>
+        <v>314</v>
+      </c>
+      <c r="B22" s="76"/>
+      <c r="C22" s="76"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H23" s="19"/>
@@ -5387,7 +5577,7 @@
       <c r="N27" s="19"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H28" s="75"/>
+      <c r="H28" s="74"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H29" s="19"/>
@@ -5440,7 +5630,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P29" type="list">
-      <formula1>$N$23:$N$27</formula1>
+      <formula1>$P$25:$P$29</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A5:C9 A10:A19 C10:C18 B14:B18 A20:C22" type="list">
@@ -5476,4 +5666,247 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="78" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="78" width="14.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="78" width="28.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="78" width="28.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="78" width="36.18"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="79" t="s">
+        <v>329</v>
+      </c>
+      <c r="B1" s="79" t="s">
+        <v>330</v>
+      </c>
+      <c r="C1" s="79" t="s">
+        <v>331</v>
+      </c>
+      <c r="D1" s="79" t="s">
+        <v>332</v>
+      </c>
+      <c r="E1" s="79" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="28.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="80"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80" t="s">
+        <v>333</v>
+      </c>
+      <c r="D2" s="81" t="s">
+        <v>334</v>
+      </c>
+      <c r="E2" s="81" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="28.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="81" t="s">
+        <v>336</v>
+      </c>
+      <c r="B3" s="81" t="s">
+        <v>337</v>
+      </c>
+      <c r="C3" s="82" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="81" t="s">
+        <v>338</v>
+      </c>
+      <c r="E3" s="81" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="36.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="81" t="s">
+        <v>336</v>
+      </c>
+      <c r="B4" s="81"/>
+      <c r="C4" s="80" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="81" t="s">
+        <v>340</v>
+      </c>
+      <c r="E4" s="81" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="28.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="81"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="80" t="s">
+        <v>342</v>
+      </c>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+    </row>
+    <row r="6" customFormat="false" ht="19.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="81"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="81"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+    </row>
+    <row r="8" customFormat="false" ht="19.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="81"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81" t="s">
+        <v>343</v>
+      </c>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+    </row>
+    <row r="9" customFormat="false" ht="37.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="81"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="81" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+    </row>
+    <row r="10" customFormat="false" ht="28.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="81" t="s">
+        <v>344</v>
+      </c>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="81"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="46.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="81"/>
+      <c r="C12" s="81" t="s">
+        <v>347</v>
+      </c>
+      <c r="D12" s="81" t="s">
+        <v>348</v>
+      </c>
+      <c r="E12" s="81" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="19.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="81" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="83"/>
+      <c r="C13" s="81" t="s">
+        <v>350</v>
+      </c>
+      <c r="D13" s="81" t="s">
+        <v>351</v>
+      </c>
+      <c r="E13" s="81" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="52.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="83"/>
+      <c r="B14" s="83"/>
+      <c r="C14" s="81" t="s">
+        <v>353</v>
+      </c>
+      <c r="D14" s="81" t="s">
+        <v>354</v>
+      </c>
+      <c r="E14" s="81"/>
+    </row>
+    <row r="15" customFormat="false" ht="19.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="83"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="81" t="s">
+        <v>353</v>
+      </c>
+      <c r="D15" s="81" t="s">
+        <v>355</v>
+      </c>
+      <c r="E15" s="81" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="21.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="81" t="s">
+        <v>357</v>
+      </c>
+      <c r="B16" s="84" t="s">
+        <v>358</v>
+      </c>
+      <c r="C16" s="85" t="s">
+        <v>125</v>
+      </c>
+      <c r="D16" s="86" t="s">
+        <v>359</v>
+      </c>
+      <c r="E16" s="81" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="87"/>
+      <c r="B17" s="87"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="83"/>
+      <c r="E17" s="87"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="87"/>
+      <c r="B18" s="87"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="87"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>